<commit_message>
Kato - Actualizare Date
</commit_message>
<xml_diff>
--- a/Database/Kato/aerlive_data.xlsx
+++ b/Database/Kato/aerlive_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\UTCN\AN III - sem 2\Practica\Script\Practica_covid19_UTCN\Database\Kato\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C401DE-DFE0-4EC6-908E-518CC48C9176}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2842D2D-8D24-48A5-9E47-E93DDCAAA0EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14088" yWindow="432" windowWidth="12588" windowHeight="11532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11916" yWindow="924" windowWidth="13152" windowHeight="11532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calitate_aerCalitate_aer (8)" sheetId="1" r:id="rId1"/>
@@ -899,15 +899,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H161"/>
+  <dimension ref="A1:H167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
       <selection activeCell="H161" sqref="H161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -5090,9 +5091,165 @@
         <v>3</v>
       </c>
       <c r="G161">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H161">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A162" s="1">
+        <v>44047</v>
+      </c>
+      <c r="B162" s="2">
+        <v>161</v>
+      </c>
+      <c r="C162">
+        <v>362</v>
+      </c>
+      <c r="D162">
+        <v>111</v>
+      </c>
+      <c r="E162">
+        <v>2</v>
+      </c>
+      <c r="F162">
+        <v>2</v>
+      </c>
+      <c r="G162">
+        <v>29</v>
+      </c>
+      <c r="H162">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A163" s="1">
+        <v>44048</v>
+      </c>
+      <c r="B163" s="2">
+        <v>162</v>
+      </c>
+      <c r="C163">
+        <v>365</v>
+      </c>
+      <c r="D163">
+        <v>106</v>
+      </c>
+      <c r="E163">
+        <v>3</v>
+      </c>
+      <c r="F163">
+        <v>3</v>
+      </c>
+      <c r="G163">
+        <v>30</v>
+      </c>
+      <c r="H163">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A164" s="1">
+        <v>44049</v>
+      </c>
+      <c r="B164" s="2">
+        <v>163</v>
+      </c>
+      <c r="C164">
+        <v>374</v>
+      </c>
+      <c r="D164">
+        <v>110</v>
+      </c>
+      <c r="E164">
+        <v>4</v>
+      </c>
+      <c r="F164">
+        <v>4</v>
+      </c>
+      <c r="G164">
+        <v>31</v>
+      </c>
+      <c r="H164">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A165" s="1">
+        <v>44050</v>
+      </c>
+      <c r="B165" s="2">
+        <v>164</v>
+      </c>
+      <c r="C165">
+        <v>388</v>
+      </c>
+      <c r="D165">
+        <v>107</v>
+      </c>
+      <c r="E165">
+        <v>5</v>
+      </c>
+      <c r="F165">
+        <v>5</v>
+      </c>
+      <c r="G165">
+        <v>29</v>
+      </c>
+      <c r="H165">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A166" s="1">
+        <v>44051</v>
+      </c>
+      <c r="B166" s="2">
+        <v>165</v>
+      </c>
+      <c r="C166">
+        <v>365</v>
+      </c>
+      <c r="D166">
+        <v>115</v>
+      </c>
+      <c r="E166">
+        <v>6</v>
+      </c>
+      <c r="F166">
+        <v>6</v>
+      </c>
+      <c r="G166">
+        <v>28</v>
+      </c>
+      <c r="H166">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A167" s="1">
+        <v>44052</v>
+      </c>
+      <c r="B167" s="2">
+        <v>166</v>
+      </c>
+      <c r="C167">
+        <v>419</v>
+      </c>
+      <c r="D167">
+        <v>109</v>
+      </c>
+      <c r="E167">
+        <v>3</v>
+      </c>
+      <c r="F167">
+        <v>3</v>
+      </c>
+      <c r="G167">
+        <v>43</v>
+      </c>
+      <c r="H167">
         <v>8</v>
       </c>
     </row>

</xml_diff>